<commit_message>
Testing and bug fixing.
</commit_message>
<xml_diff>
--- a/changepoint/tests/cpt.xlsx
+++ b/changepoint/tests/cpt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alix\Documents\changepoint_python\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alix\Documents\changepoint_python\changepoint\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="B2:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>1</v>
@@ -642,7 +642,7 @@
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>2</v>
@@ -693,7 +693,7 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>5</v>

</xml_diff>